<commit_message>
updated the sheetname as per feedback
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="DemonstrationTest" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -47,7 +47,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -56,17 +56,12 @@
     <font>
       <b/>
       <sz val="8.0"/>
-      <name val="Cambria"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
       <sz val="8.0"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-    </font>
-    <font/>
-    <font>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -102,24 +97,27 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -361,13 +359,13 @@
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>